<commit_message>
UPDATE LAYOUT MASTER BARANG SATU SATUAN
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangSatuSatuan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangSatuSatuan.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,40 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCCA0D27-7E92-4247-9929-721D7D9DF711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A1F3D2-F7E0-423A-8D28-6FD7A953A37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>NAMABARANG</t>
   </si>
   <si>
-    <t>JENISBARANG</t>
-  </si>
-  <si>
-    <t>MERKBARANG</t>
-  </si>
-  <si>
     <t>SATUAN</t>
   </si>
   <si>
@@ -61,12 +44,72 @@
   </si>
   <si>
     <t>JMLBARANG</t>
+  </si>
+  <si>
+    <t>KOPI</t>
+  </si>
+  <si>
+    <t>GULAKU</t>
+  </si>
+  <si>
+    <t>MAKARONI</t>
+  </si>
+  <si>
+    <t>MINUMAN</t>
+  </si>
+  <si>
+    <t>BAHAN MASAKAN</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>KATEGORI</t>
+  </si>
+  <si>
+    <t>SUBKATEGORI</t>
+  </si>
+  <si>
+    <t>PCS</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>TEH JAWA</t>
+  </si>
+  <si>
+    <t>32140P</t>
+  </si>
+  <si>
+    <t>H09327392</t>
+  </si>
+  <si>
+    <t>P4387439</t>
+  </si>
+  <si>
+    <t>J0923742</t>
+  </si>
+  <si>
+    <t>UDI JAYA</t>
+  </si>
+  <si>
+    <t>BUDI LUHUR</t>
+  </si>
+  <si>
+    <t>RAK 1</t>
+  </si>
+  <si>
+    <t>RAK 2</t>
+  </si>
+  <si>
+    <t>RAK 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -153,7 +196,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -173,12 +216,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -461,11 +498,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -483,127 +520,165 @@
     <col min="12" max="12" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6">
+        <v>5000</v>
+      </c>
+      <c r="F2" s="6">
+        <v>6500</v>
+      </c>
+      <c r="G2" s="6">
+        <v>30</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6">
+        <v>7500</v>
+      </c>
+      <c r="F3" s="6">
+        <v>9000</v>
+      </c>
+      <c r="G3" s="6">
+        <v>40</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6">
+        <v>15000</v>
+      </c>
+      <c r="F4" s="6">
+        <v>17000</v>
+      </c>
+      <c r="G4" s="6">
+        <v>50</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>28000</v>
+      </c>
+      <c r="G5" s="6">
+        <v>50</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="256" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>